<commit_message>
UserStories korrigiert von Marvin
</commit_message>
<xml_diff>
--- a/planning/UserStoriesFlattie.xlsx
+++ b/planning/UserStoriesFlattie.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TBZ\M426 Methoden zu Softwareentwicklung Rollen Aufgaben Ergebnisse\wgapp\FlatsharePlanner\planning\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -48,9 +53,6 @@
     <t>As a user, I want to be able to throw a member out of my Flattie group, so that flat members which don't live in our flat anymore cannot see the flat internal information anymore.</t>
   </si>
   <si>
-    <t>As a user, I want to be able to throw myself out of a Flattie group, so that I cannot see the flat internal information anymore.</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to add a calendar entry, so that every Flattie group member can see my entry in the shared calendar.</t>
   </si>
   <si>
@@ -63,33 +65,15 @@
     <t>As a user, I want to be able to delete a calendar entry, so that an unnessessary or cancelled event isn't distracting from the real events.</t>
   </si>
   <si>
-    <t>As a user, I want to be able to add a repeatable event into the shared calendar, so that I don't have to enter same event multiple times manually.</t>
-  </si>
-  <si>
-    <t>As a user, I want to be able to delete a repeatable event, so that I don't have to delete same event multiple times manually.</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to delete one entry of a repeatable event, so that I can delete exceptions from the repeatable events.</t>
   </si>
   <si>
     <t>As a user, I want to be able to update a calendar entry, so that event changes can be entered in the calendar.</t>
   </si>
   <si>
-    <t>As a user, I want to be able to update a repeatable event, so that I don't have to change same event information multiple times manually.</t>
-  </si>
-  <si>
-    <t>As a user, I want to be able to update one entry of a repeatable event, so that I can enter exceptions from the repeatable events.</t>
-  </si>
-  <si>
-    <t>As a user, I want to be able to assign a calendar event to a Flattie group member, so that all Flattie group members can see who is responsable for the event (especially important for duties).</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to see our Flattie shopping list, so that I can see what groceries and other stuff need to be bought.</t>
   </si>
   <si>
-    <t>As a user, I want to be able to add an item to the shopping list, so that the needed item will get bought by anyone.</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to mark an item of the shopping list, so that every flat member sees that I am going to buy this item.</t>
   </si>
   <si>
@@ -127,12 +111,33 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want to be able to throw myself out of a Flattie group, so that I can join or create another group. </t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to add a repeatable event into the shared calendar, so that I don't have to enter same events multiple times manually.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to delete a repeatable event, so that I don't have to delete same events multiple times manually.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to update a repeatable event, so that I don't have to change the same event information multiple times manually.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to update one entry of a repeatable event, so that I can enter exceptions for the repeatable event.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to assign a calendar event to a Flattie group member, so that all Flattie group members can see who is responsible for the event (especially important for duties).</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to add an item to the shopping list, so that the needed item will get bought by a member of the group.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,32 +553,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="13" customWidth="1"/>
-    <col min="4" max="5" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6.85546875" style="13" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="4.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" style="13" customWidth="1"/>
+    <col min="4" max="5" width="6.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.88671875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -584,7 +589,7 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -593,25 +598,25 @@
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -620,7 +625,7 @@
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -628,7 +633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -636,12 +641,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -649,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -657,7 +662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -665,100 +670,100 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>17</v>
       </c>
@@ -766,62 +771,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>